<commit_message>
New tree names added
</commit_message>
<xml_diff>
--- a/Data_Sources/Tree_Name_mapping.xlsx
+++ b/Data_Sources/Tree_Name_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opilane\Desktop\Andmetarkus,git\Andmetarkus\Timber AS\Timber-AS\Data_Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{194112B3-4865-40E0-98AA-612FE1F14F04}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B60BA280-1BF0-4E65-B291-391667BE33DF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{F791A6DC-4537-46A0-9938-B0BDE1941023}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>MA</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Name_ENG</t>
+  </si>
+  <si>
+    <t>spruce</t>
+  </si>
+  <si>
+    <t>birch</t>
   </si>
 </sst>
 </file>
@@ -477,7 +483,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,10 +511,16 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Py uploading latest version
</commit_message>
<xml_diff>
--- a/Data_Sources/Tree_Name_mapping.xlsx
+++ b/Data_Sources/Tree_Name_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\opilane\Desktop\Andmetarkus,git\Andmetarkus\Timber AS\Timber-AS\Data_Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528ADBE8-D852-4A3D-914C-E2438D3442CB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34439F21-EF6A-4DDB-8967-E0F1C67BAB34}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6810" xr2:uid="{F791A6DC-4537-46A0-9938-B0BDE1941023}"/>
   </bookViews>
@@ -93,22 +93,22 @@
     <t>TL</t>
   </si>
   <si>
-    <t>pine</t>
-  </si>
-  <si>
     <t>Name_EE</t>
   </si>
   <si>
     <t>Name_ENG</t>
   </si>
   <si>
-    <t>spruce</t>
-  </si>
-  <si>
-    <t>birch</t>
-  </si>
-  <si>
-    <t>other_deciduous</t>
+    <t>Pine</t>
+  </si>
+  <si>
+    <t>Spruce</t>
+  </si>
+  <si>
+    <t>Birch</t>
+  </si>
+  <si>
+    <t>Other Deciduous</t>
   </si>
 </sst>
 </file>
@@ -496,10 +496,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" t="s">
         <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -507,7 +507,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>